<commit_message>
Add jumper config photo
</commit_message>
<xml_diff>
--- a/isg-clock-generator-rev1/PCBA-tracking-isg-clock-generator-rev1.xlsx
+++ b/isg-clock-generator-rev1/PCBA-tracking-isg-clock-generator-rev1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/github/dkramnik/Eagle-Public/isg-clock-generator-rev1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35237DA4-9D5C-7F46-8147-3F2FCCCAE0F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9692D91A-FAD4-D240-9646-7F526C05D53A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="2000" windowWidth="28040" windowHeight="17440" xr2:uid="{D16C10D5-49C1-B84C-951E-E0C13C5C72CA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Board ID</t>
   </si>
@@ -45,12 +45,6 @@
     <t>C34/C35</t>
   </si>
   <si>
-    <t>R22/R24</t>
-  </si>
-  <si>
-    <t>R23/R25</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -94,6 +88,21 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>R23/R25 (Pullup to 1.8V)</t>
+  </si>
+  <si>
+    <t>R22/R24 (Pulldown to GND)</t>
+  </si>
+  <si>
+    <t>DC Bias [V]</t>
+  </si>
+  <si>
+    <t>1nF</t>
+  </si>
+  <si>
+    <t>DNP</t>
   </si>
 </sst>
 </file>
@@ -137,9 +146,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,18 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D045639F-BA91-6641-806E-7194123840C9}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,122 +490,138 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>615</v>
+      </c>
+      <c r="E2">
+        <v>690</v>
+      </c>
+      <c r="F2" s="3">
+        <f>1.8*D2/(D2+E2)</f>
+        <v>0.84827586206896555</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
+      <c r="H4" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
+      <c r="H5" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>